<commit_message>
update budget with actuals
</commit_message>
<xml_diff>
--- a/Budget/owasp-summit-2017-budget with actuals v20170506.xlsx
+++ b/Budget/owasp-summit-2017-budget with actuals v20170506.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="readme1st" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="128">
   <si>
     <t>Estimated profit</t>
   </si>
@@ -299,12 +299,6 @@
     <t>GBP TO USD</t>
   </si>
   <si>
-    <t>continuum</t>
-  </si>
-  <si>
-    <t>Axa Assistance</t>
-  </si>
-  <si>
     <t>PBX</t>
   </si>
   <si>
@@ -408,6 +402,15 @@
   </si>
   <si>
     <t>Catering (70 p full)</t>
+  </si>
+  <si>
+    <t>1und1 - daniel</t>
+  </si>
+  <si>
+    <t>continuum - stephen</t>
+  </si>
+  <si>
+    <t>Axa Assistance - Marc</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -802,13 +805,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1124,7 +1130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B33" sqref="B33:F39"/>
     </sheetView>
   </sheetViews>
@@ -1154,10 +1160,10 @@
     </row>
     <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="78"/>
+      <c r="C2" s="80"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="66" t="s">
@@ -1624,12 +1630,12 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C33" s="63"/>
       <c r="D33" s="8"/>
       <c r="E33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="33"/>
@@ -1638,7 +1644,7 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C34" s="63">
         <f>sponsored!C14</f>
@@ -1646,9 +1652,9 @@
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F34" s="79">
+        <v>110</v>
+      </c>
+      <c r="F34" s="78">
         <f>19330*invoiced!H1</f>
         <v>25129</v>
       </c>
@@ -1667,9 +1673,9 @@
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F35" s="79">
+        <v>111</v>
+      </c>
+      <c r="F35" s="78">
         <f>41250*invoiced!H1</f>
         <v>53625</v>
       </c>
@@ -1680,19 +1686,19 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C36" s="63">
         <f>invoiced!C13</f>
-        <v>20358</v>
+        <v>21918</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F36" s="79">
+        <v>124</v>
+      </c>
+      <c r="F36" s="78">
         <f>catering!B8*totals!B9</f>
-        <v>28437.5</v>
+        <v>28843.75</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="33"/>
@@ -1703,13 +1709,13 @@
       <c r="B37" s="8"/>
       <c r="C37" s="63">
         <f>SUM(C34:C36)</f>
-        <v>84190.8</v>
+        <v>85750.8</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="79">
+      <c r="F37" s="78">
         <f>SUM(F34:F36)</f>
-        <v>107191.5</v>
+        <v>107597.75</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="33"/>
@@ -1732,11 +1738,11 @@
       <c r="C39" s="63"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F39" s="79">
+        <v>123</v>
+      </c>
+      <c r="F39" s="78">
         <f>C37-F37</f>
-        <v>-23000.699999999997</v>
+        <v>-21846.949999999997</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="33"/>
@@ -2184,15 +2190,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2">
         <f>4.75*invoiced!H1</f>
@@ -2201,7 +2207,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <f>16*invoiced!H1</f>
@@ -2210,7 +2216,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4">
         <f>33*invoiced!H1</f>
@@ -2219,7 +2225,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>8.75*invoiced!H1</f>
@@ -2228,7 +2234,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7">
         <f>SUM(B2:B6)</f>
@@ -2237,7 +2243,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8">
         <f>5*B7</f>
@@ -2727,14 +2733,14 @@
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2">
         <f>sponsored!B14</f>
@@ -2743,7 +2749,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3">
         <f>tickets!A2</f>
@@ -2752,16 +2758,16 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4">
         <f>invoiced!B13</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -2769,7 +2775,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -2777,11 +2783,11 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9">
         <f>SUM(B2:B8)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2805,13 +2811,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" t="s">
-        <v>107</v>
       </c>
       <c r="I1">
         <v>1.1000000000000001</v>
@@ -2835,13 +2841,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="B13:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2876,7 +2882,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2888,7 +2894,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2900,7 +2906,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -2910,14 +2916,26 @@
         <v>9984</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="77">
+        <f>1200*H1</f>
+        <v>1560</v>
+      </c>
+    </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="76">
         <f>SUM(B2:B12)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <f>SUM(C2:C12)</f>
-        <v>20358</v>
+        <v>21918</v>
       </c>
     </row>
   </sheetData>
@@ -2943,18 +2961,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>87</v>
       </c>
       <c r="C1" s="67" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="67">
         <v>2</v>
@@ -2965,7 +2983,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="67" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" s="67">
         <v>0</v>
@@ -2976,7 +2994,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="67" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" s="67">
         <v>0</v>
@@ -2987,7 +3005,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="67" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="67">
         <v>4</v>
@@ -2998,7 +3016,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="67" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="67">
         <v>2</v>
@@ -3009,7 +3027,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="67" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="67">
         <v>1</v>
@@ -3018,12 +3036,12 @@
         <v>4000</v>
       </c>
       <c r="D7" s="67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" s="67">
         <v>2</v>
@@ -3032,12 +3050,12 @@
         <v>3900</v>
       </c>
       <c r="D8" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="67" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="67">
         <v>0</v>

</xml_diff>